<commit_message>
Dukientruythu Dukienthuenam truythu thue
</commit_message>
<xml_diff>
--- a/data/MauExample/DuKienThueCuaNam_7010905002_2015.xlsx
+++ b/data/MauExample/DuKienThueCuaNam_7010905002_2015.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>STT</t>
   </si>
@@ -265,12 +265,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -278,6 +272,12 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
@@ -581,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +595,7 @@
     <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
     <col min="5" max="5" width="22.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="25" customWidth="1"/>
+    <col min="7" max="7" width="23" style="23" customWidth="1"/>
     <col min="8" max="8" width="23" style="2" customWidth="1"/>
     <col min="9" max="9" width="23" style="9" customWidth="1"/>
     <col min="10" max="11" width="23" style="6" customWidth="1"/>
@@ -604,51 +604,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -669,7 +669,7 @@
       <c r="F4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -702,22 +702,24 @@
         <v>15</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" s="15">
-        <v>8500000</v>
-      </c>
-      <c r="F5" s="19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G5" s="24">
-        <v>1</v>
-      </c>
-      <c r="H5" s="17"/>
+        <v>6800000</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="I5" s="16"/>
-      <c r="J5" s="15"/>
+      <c r="J5" s="15">
+        <v>3800000</v>
+      </c>
       <c r="K5" s="15">
-        <v>42500</v>
+        <v>2850000</v>
       </c>
       <c r="L5" s="17" t="s">
         <v>27</v>
@@ -730,29 +732,23 @@
       <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="15">
-        <v>8500000</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="G6" s="24">
-        <v>1</v>
-      </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15">
-        <v>85000</v>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>9300000</v>
+      </c>
+      <c r="F6" s="20">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K6" s="6">
+        <v>46500</v>
       </c>
       <c r="L6" s="17" t="s">
         <v>27</v>
@@ -765,31 +761,23 @@
       <c r="A7" s="12">
         <v>3</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="15">
-        <v>6800000</v>
-      </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="24">
-        <v>0.75</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="15">
-        <v>3800000</v>
-      </c>
-      <c r="K7" s="15">
-        <v>2850000</v>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9300000</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="6">
+        <v>93000</v>
       </c>
       <c r="L7" s="17" t="s">
         <v>27</v>
@@ -799,7 +787,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="12">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -809,16 +797,19 @@
         <v>17</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6">
-        <v>9300000</v>
-      </c>
-      <c r="F8" s="20">
-        <v>5.0000000000000001E-3</v>
+        <v>26</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="6">
+        <v>3000</v>
       </c>
       <c r="K8" s="6">
-        <v>46500</v>
+        <v>3000000</v>
       </c>
       <c r="L8" s="17" t="s">
         <v>27</v>
@@ -828,26 +819,30 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="12">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6">
-        <v>9300000</v>
-      </c>
-      <c r="F9" s="20">
-        <v>0.01</v>
-      </c>
-      <c r="K9" s="6">
-        <v>93000</v>
+      <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="15">
+        <v>10400000</v>
+      </c>
+      <c r="F9" s="19">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15">
+        <v>52000</v>
       </c>
       <c r="L9" s="17" t="s">
         <v>27</v>
@@ -857,29 +852,30 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="12">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="9">
-        <v>1000</v>
-      </c>
-      <c r="J10" s="6">
-        <v>3000</v>
-      </c>
-      <c r="K10" s="6">
-        <v>3000000</v>
+      <c r="B10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="15">
+        <v>10400000</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15">
+        <v>104000</v>
       </c>
       <c r="L10" s="17" t="s">
         <v>27</v>
@@ -899,21 +895,23 @@
         <v>19</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="15">
-        <v>10400000</v>
-      </c>
-      <c r="F11" s="19">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15">
-        <v>52000</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="22">
+        <v>0.12</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="16">
+        <v>100</v>
+      </c>
+      <c r="J11" s="15">
+        <v>700000</v>
+      </c>
+      <c r="K11" s="15"/>
       <c r="L11" s="17" t="s">
         <v>27</v>
       </c>
@@ -925,27 +923,23 @@
       <c r="A12" s="12">
         <v>8</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="15">
-        <v>10400000</v>
-      </c>
-      <c r="F12" s="19">
-        <v>0.01</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15">
-        <v>104000</v>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6">
+        <v>9700000</v>
+      </c>
+      <c r="F12" s="20">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K12" s="6">
+        <v>48500</v>
       </c>
       <c r="L12" s="17" t="s">
         <v>27</v>
@@ -958,92 +952,28 @@
       <c r="A13" s="12">
         <v>9</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="24">
-        <v>0.12</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="16">
-        <v>100</v>
-      </c>
-      <c r="J13" s="15">
-        <v>700000</v>
-      </c>
-      <c r="K13" s="15"/>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6">
+        <v>9700000</v>
+      </c>
+      <c r="F13" s="20">
+        <v>0.01</v>
+      </c>
+      <c r="K13" s="6">
+        <v>97000</v>
+      </c>
       <c r="L13" s="17" t="s">
         <v>27</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="6">
-        <v>9700000</v>
-      </c>
-      <c r="F14" s="20">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="K14" s="6">
-        <v>48500</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6">
-        <v>9700000</v>
-      </c>
-      <c r="F15" s="20">
-        <v>0.01</v>
-      </c>
-      <c r="K15" s="6">
-        <v>97000</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15" s="17" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>